<commit_message>
modified code in excel reader
</commit_message>
<xml_diff>
--- a/src/main/resources/Test.xlsx
+++ b/src/main/resources/Test.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21705"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37C3A04A-4E05-49F6-9659-071AAADD327C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14325" windowHeight="4500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A2:N14"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>in1</t>
   </si>
@@ -42,12 +42,15 @@
   </si>
   <si>
     <t>op3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -139,7 +142,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -191,7 +194,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -385,18 +388,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -422,11 +425,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EAAE743-92B2-4B2F-877A-42C590999145}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{2ABD6402-0D3A-5A7B-9ACA-3C34C81507D6}">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -435,9 +438,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <f>Sheet1!B3*2</f>
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">

</xml_diff>

<commit_message>
modified code to read from json also created new files
</commit_message>
<xml_diff>
--- a/src/main/resources/Test.xlsx
+++ b/src/main/resources/Test.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14325" windowHeight="4500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15900" windowHeight="4290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A2:N14"/>
+  <oleSize ref="A1:P12"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>in1</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>op3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -388,7 +385,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -396,27 +393,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:A5"/>
+  <dimension ref="A3:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -428,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -438,8 +444,9 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="B2">
+        <f>Sheet1!B3+2</f>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -448,7 +455,7 @@
       </c>
       <c r="B3">
         <f>Sheet1!B4*5</f>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -457,7 +464,7 @@
       </c>
       <c r="B4">
         <f>Sheet1!B5+Sheet1!B4+Sheet1!B3</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>